<commit_message>
diff changes 1.48 and 1.49
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Intra_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Intra_State.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/Excel Template new/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,9 +32,6 @@
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
   <si>
-    <t>92C/1, LANE 7, EAST AZAD NAGAR, KRISHNA NAGAR, DELHI 110051</t>
-  </si>
-  <si>
     <t>({meta:recipient_type})</t>
   </si>
   <si>
@@ -199,12 +196,16 @@
   </si>
   <si>
     <t>Reverse Charge: No</t>
+  </si>
+  <si>
+    <t>A-1/7a, A BLOCK, KRISHNA NAGAR, 
+DELHI 110051</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,72 +967,100 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1042,50 +1071,45 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1095,55 +1119,32 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,6 +1154,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1175,7 +1179,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.png"/>
+        <xdr:cNvPr id="2" name="image1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1212,7 +1222,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image2.jpg" title="Image"/>
+        <xdr:cNvPr id="3" name="image2.jpg" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1249,7 +1265,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="4" name="image3.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1540,7 +1562,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:S10"/>
+      <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1589,742 +1611,742 @@
     </row>
     <row r="2" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="43"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
     </row>
     <row r="3" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="S3" s="63"/>
+      <c r="S3" s="24"/>
     </row>
     <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="62"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="85" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="63"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="24"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="63"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="24"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="84" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="43"/>
+      <c r="B6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="64"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="43"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="19"/>
     </row>
     <row r="9" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="74"/>
+      <c r="B9" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="80"/>
     </row>
     <row r="10" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="18"/>
+      <c r="B10" s="91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="92"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="15"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="90"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="38"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="72"/>
     </row>
     <row r="13" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="40"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="73"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="82"/>
+      <c r="D14" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22" t="s">
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="S14" s="74"/>
+      <c r="S14" s="80"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="29" t="s">
+      <c r="I15" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="J15" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="K15" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="L15" s="48"/>
+      <c r="M15" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="32"/>
-      <c r="M15" s="27" t="s">
+      <c r="N15" s="65"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="27" t="s">
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="97" t="s">
         <v>24</v>
-      </c>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="34"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="100"/>
+      <c r="L16" s="77"/>
       <c r="M16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="24"/>
+        <v>20</v>
+      </c>
+      <c r="N16" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" s="63"/>
       <c r="P16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="24"/>
-      <c r="S16" s="26"/>
+        <v>20</v>
+      </c>
+      <c r="Q16" s="96" t="s">
+        <v>25</v>
+      </c>
+      <c r="R16" s="63"/>
+      <c r="S16" s="98"/>
     </row>
     <row r="17" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="J17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="73" t="s">
+      <c r="L17" s="41"/>
+      <c r="M17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="69"/>
-      <c r="M17" s="5" t="s">
+      <c r="N17" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="N17" s="73" t="s">
+      <c r="O17" s="41"/>
+      <c r="P17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="69"/>
-      <c r="P17" s="5" t="s">
+      <c r="Q17" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="73" t="s">
+      <c r="R17" s="41"/>
+      <c r="S17" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="R17" s="69"/>
-      <c r="S17" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="71"/>
+      <c r="B18" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="8"/>
       <c r="I18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="35" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="32"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="35" t="s">
+      <c r="O18" s="48"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="32"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="35" t="s">
+      <c r="R18" s="48"/>
+      <c r="S18" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="R18" s="32"/>
-      <c r="S18" s="12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="L19" s="90"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="90"/>
-      <c r="O19" s="90"/>
-      <c r="P19" s="90"/>
-      <c r="Q19" s="90"/>
-      <c r="R19" s="91"/>
-      <c r="S19" s="92" t="s">
-        <v>38</v>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="93"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="93"/>
-      <c r="P20" s="93"/>
-      <c r="Q20" s="93"/>
-      <c r="R20" s="94"/>
-      <c r="S20" s="95" t="s">
-        <v>39</v>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="93"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="93"/>
-      <c r="R21" s="94"/>
-      <c r="S21" s="95" t="s">
-        <v>40</v>
+      <c r="B21" s="22"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="55" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="56"/>
+      <c r="S22" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="97"/>
-      <c r="S22" s="98" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="96"/>
-      <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-      <c r="S23" s="99">
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="43"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="19"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="52"/>
+      <c r="B25" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="60"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="43"/>
+      <c r="B26" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="19"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="62"/>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="63"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="24"/>
     </row>
     <row r="28" spans="1:19" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="62"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="62"/>
-      <c r="R28" s="62"/>
-      <c r="S28" s="63"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="24"/>
     </row>
     <row r="29" spans="1:19" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="48"/>
-      <c r="S29" s="64"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="22"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="31"/>
+    </row>
+    <row r="30" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="64"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="31"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
@@ -2349,39 +2371,14 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="R3:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:S7"/>
-    <mergeCell ref="G4:Q4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="F3:Q3"/>
-    <mergeCell ref="B20:J22"/>
-    <mergeCell ref="K19:R19"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K20:R20"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="K26:S29"/>
-    <mergeCell ref="K30:S30"/>
-    <mergeCell ref="K22:R22"/>
-    <mergeCell ref="K24:S25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="K23:R23"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="H23:J30"/>
-    <mergeCell ref="B27:G30"/>
-    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S15:S16"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:L16"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="D12:S13"/>
     <mergeCell ref="K8:S8"/>
@@ -2398,14 +2395,39 @@
     <mergeCell ref="B10:S10"/>
     <mergeCell ref="D14:H14"/>
     <mergeCell ref="I14:Q14"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S15:S16"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K26:S29"/>
+    <mergeCell ref="K30:S30"/>
+    <mergeCell ref="K22:R22"/>
+    <mergeCell ref="K24:S25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="H23:J30"/>
+    <mergeCell ref="B27:G30"/>
+    <mergeCell ref="B6:S7"/>
+    <mergeCell ref="G4:Q4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="F3:Q3"/>
+    <mergeCell ref="B20:J22"/>
+    <mergeCell ref="K19:R19"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="R3:S4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
In the Invoice Anx meta data tcs issue in the excel sheet #CRMS-1924
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/247around_Tax_Invoice_Intra_State.xlsx
+++ b/application/controllers/excel-templates/247around_Tax_Invoice_Intra_State.xlsx
@@ -168,7 +168,7 @@
     <t xml:space="preserve">{meta:tcs_rate_text}				</t>
   </si>
   <si>
-    <t>{meta:tds_mount}</t>
+    <t>{meta:tcs_mount}</t>
   </si>
   <si>
     <t>Total Amount</t>
@@ -314,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="50">
     <border/>
     <border>
       <left style="medium">
@@ -743,13 +743,6 @@
       <bottom/>
     </border>
     <border>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -767,27 +760,12 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -951,7 +929,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -972,14 +950,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="29" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -988,26 +966,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="47" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf borderId="8" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="49" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="48" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="53" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="49" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1820,11 +1791,11 @@
       <c r="D25" s="87"/>
       <c r="E25" s="87"/>
       <c r="F25" s="87"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="89"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="88"/>
       <c r="I25" s="3"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="90" t="s">
+      <c r="K25" s="84" t="s">
         <v>55</v>
       </c>
       <c r="L25" s="14"/>
@@ -1834,7 +1805,7 @@
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
-      <c r="S25" s="91">
+      <c r="S25" s="89">
         <v>0.0</v>
       </c>
     </row>
@@ -1850,7 +1821,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="10"/>
       <c r="J26" s="9"/>
-      <c r="K26" s="92" t="s">
+      <c r="K26" s="90" t="s">
         <v>57</v>
       </c>
       <c r="L26" s="3"/>
@@ -1864,39 +1835,32 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="93" t="s">
+      <c r="B27" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
       <c r="G27" s="60"/>
       <c r="H27" s="10"/>
       <c r="J27" s="9"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="96"/>
-      <c r="M27" s="96"/>
-      <c r="N27" s="96"/>
-      <c r="O27" s="96"/>
-      <c r="P27" s="96"/>
-      <c r="Q27" s="96"/>
-      <c r="R27" s="96"/>
-      <c r="S27" s="97"/>
+      <c r="K27" s="10"/>
+      <c r="S27" s="9"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="93" t="s">
+      <c r="B28" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="60"/>
       <c r="H28" s="10"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="89"/>
+      <c r="K28" s="88"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -1908,7 +1872,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="89"/>
+      <c r="B29" s="88"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1955,7 +1919,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="14"/>
       <c r="J32" s="19"/>
-      <c r="K32" s="98" t="s">
+      <c r="K32" s="93" t="s">
         <v>60</v>
       </c>
       <c r="L32" s="14"/>
@@ -2955,7 +2919,6 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="60">
     <mergeCell ref="I16:I17"/>
@@ -2972,15 +2935,15 @@
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K28:S31"/>
+    <mergeCell ref="K32:S32"/>
     <mergeCell ref="K20:R20"/>
     <mergeCell ref="K21:R21"/>
     <mergeCell ref="K22:R22"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K24:R24"/>
     <mergeCell ref="K25:R25"/>
     <mergeCell ref="K26:S27"/>
-    <mergeCell ref="K28:S31"/>
-    <mergeCell ref="K32:S32"/>
     <mergeCell ref="G5:Q5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="B2:S2"/>
@@ -3013,11 +2976,11 @@
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:J20"/>
+    <mergeCell ref="B21:J24"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="H25:J32"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="B29:G32"/>
-    <mergeCell ref="B21:J24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins bottom="0.25" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.25"/>

</xml_diff>